<commit_message>
Added 3 new czech books
</commit_message>
<xml_diff>
--- a/docs/albituzka_soft.xlsx
+++ b/docs/albituzka_soft.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A35BCDB-0E8C-45B9-B0E5-A3F1C7DA912C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC168FE-47C5-4E0C-877D-394090268563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2350" uniqueCount="1244">
   <si>
     <t>Lang</t>
   </si>
@@ -3699,6 +3699,54 @@
   </si>
   <si>
     <t>96kbps CBR stereo/44.1kHz: 83%</t>
+  </si>
+  <si>
+    <t>3493-kvido-dvoulist.bnl</t>
+  </si>
+  <si>
+    <t>060cc9b5afe16788e2d1fe5f5ba8f12b</t>
+  </si>
+  <si>
+    <t>0x00000DA5</t>
+  </si>
+  <si>
+    <t>0x2EE1</t>
+  </si>
+  <si>
+    <t>0x002C</t>
+  </si>
+  <si>
+    <t>128kbps CBR stereo/44.1kHz: 86%</t>
+  </si>
+  <si>
+    <t>anglictina-pro-samouky-3328.bnl</t>
+  </si>
+  <si>
+    <t>8b89c922c0c1588c3710cfca45064413</t>
+  </si>
+  <si>
+    <t>0x00000D00</t>
+  </si>
+  <si>
+    <t>0x4255</t>
+  </si>
+  <si>
+    <t>0x22EF</t>
+  </si>
+  <si>
+    <t>casopis6-3336.bnl</t>
+  </si>
+  <si>
+    <t>643d0232aad369d8c59aa800e507ad69</t>
+  </si>
+  <si>
+    <t>0x00000D08</t>
+  </si>
+  <si>
+    <t>0x2F4D</t>
+  </si>
+  <si>
+    <t>0x045C</t>
   </si>
 </sst>
 </file>
@@ -3772,8 +3820,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J258" totalsRowShown="0">
-  <autoFilter ref="A1:J258" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J261" totalsRowShown="0">
+  <autoFilter ref="A1:J261" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J261">
+    <sortCondition ref="E1:E261"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Lang"/>
@@ -4111,10 +4162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J258"/>
+  <dimension ref="A1:J261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A244" sqref="A244"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="J262" sqref="J262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12384,6 +12435,102 @@
         <v>1227</v>
       </c>
     </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C259" s="2">
+        <v>463397888</v>
+      </c>
+      <c r="D259" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E259" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="F259" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="G259" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H259" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="I259" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="J259" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C260" s="2">
+        <v>100908544</v>
+      </c>
+      <c r="D260" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E260" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="F260" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G260" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H260" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="I260" s="3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="J260" s="4" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C261" s="2">
+        <v>14982656</v>
+      </c>
+      <c r="D261" s="3" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E261" s="3" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F261" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G261" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H261" s="3" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I261" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="J261" s="4" t="s">
+        <v>1233</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>